<commit_message>
Modifications with Unit Value
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/ITC_Trade_Data/841810_CHN_all.xlsx
+++ b/Data_Sources_and_Preparation/ITC_Trade_Data/841810_CHN_all.xlsx
@@ -488,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM142"/>
+  <dimension ref="A1:AM145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16960,6 +16960,363 @@
         <v>8118</v>
       </c>
     </row>
+    <row r="143" spans="1:39">
+      <c r="A143">
+        <v>10737</v>
+      </c>
+      <c r="B143">
+        <v>202486</v>
+      </c>
+      <c r="C143">
+        <v>27930</v>
+      </c>
+      <c r="D143">
+        <v>36513</v>
+      </c>
+      <c r="E143">
+        <v>7910</v>
+      </c>
+      <c r="F143">
+        <v>8520</v>
+      </c>
+      <c r="G143">
+        <v>201801</v>
+      </c>
+      <c r="H143">
+        <v>2018</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>11329</v>
+      </c>
+      <c r="K143">
+        <v>16218</v>
+      </c>
+      <c r="L143">
+        <v>17063</v>
+      </c>
+      <c r="M143">
+        <v>13762</v>
+      </c>
+      <c r="N143">
+        <v>12786</v>
+      </c>
+      <c r="O143">
+        <v>201919</v>
+      </c>
+      <c r="P143">
+        <v>218433</v>
+      </c>
+      <c r="Q143">
+        <v>206469</v>
+      </c>
+      <c r="R143">
+        <v>250030</v>
+      </c>
+      <c r="S143">
+        <v>173270</v>
+      </c>
+      <c r="T143">
+        <v>30844</v>
+      </c>
+      <c r="U143">
+        <v>35783</v>
+      </c>
+      <c r="V143">
+        <v>39061</v>
+      </c>
+      <c r="W143">
+        <v>34123</v>
+      </c>
+      <c r="X143">
+        <v>29779</v>
+      </c>
+      <c r="Y143">
+        <v>18014</v>
+      </c>
+      <c r="Z143">
+        <v>21023</v>
+      </c>
+      <c r="AA143">
+        <v>13724</v>
+      </c>
+      <c r="AB143">
+        <v>41151</v>
+      </c>
+      <c r="AC143">
+        <v>20518</v>
+      </c>
+      <c r="AD143">
+        <v>12252</v>
+      </c>
+      <c r="AE143">
+        <v>9481</v>
+      </c>
+      <c r="AF143">
+        <v>10964</v>
+      </c>
+      <c r="AG143">
+        <v>14366</v>
+      </c>
+      <c r="AH143">
+        <v>7691</v>
+      </c>
+      <c r="AI143">
+        <v>12027</v>
+      </c>
+      <c r="AJ143">
+        <v>9489</v>
+      </c>
+      <c r="AK143">
+        <v>11640</v>
+      </c>
+      <c r="AL143">
+        <v>6686</v>
+      </c>
+      <c r="AM143">
+        <v>8432</v>
+      </c>
+    </row>
+    <row r="144" spans="1:39">
+      <c r="A144">
+        <v>11788</v>
+      </c>
+      <c r="B144">
+        <v>191772</v>
+      </c>
+      <c r="C144">
+        <v>23639</v>
+      </c>
+      <c r="D144">
+        <v>20320</v>
+      </c>
+      <c r="E144">
+        <v>6642</v>
+      </c>
+      <c r="F144">
+        <v>7276</v>
+      </c>
+      <c r="G144">
+        <v>201802</v>
+      </c>
+      <c r="H144">
+        <v>2018</v>
+      </c>
+      <c r="I144">
+        <v>2</v>
+      </c>
+      <c r="J144">
+        <v>10737</v>
+      </c>
+      <c r="K144">
+        <v>11329</v>
+      </c>
+      <c r="L144">
+        <v>16218</v>
+      </c>
+      <c r="M144">
+        <v>17149</v>
+      </c>
+      <c r="N144">
+        <v>12007</v>
+      </c>
+      <c r="O144">
+        <v>202486</v>
+      </c>
+      <c r="P144">
+        <v>201919</v>
+      </c>
+      <c r="Q144">
+        <v>218433</v>
+      </c>
+      <c r="R144">
+        <v>246910</v>
+      </c>
+      <c r="S144">
+        <v>175086</v>
+      </c>
+      <c r="T144">
+        <v>27930</v>
+      </c>
+      <c r="U144">
+        <v>30844</v>
+      </c>
+      <c r="V144">
+        <v>35783</v>
+      </c>
+      <c r="W144">
+        <v>36842</v>
+      </c>
+      <c r="X144">
+        <v>24395</v>
+      </c>
+      <c r="Y144">
+        <v>36513</v>
+      </c>
+      <c r="Z144">
+        <v>18014</v>
+      </c>
+      <c r="AA144">
+        <v>21023</v>
+      </c>
+      <c r="AB144">
+        <v>28446</v>
+      </c>
+      <c r="AC144">
+        <v>26540</v>
+      </c>
+      <c r="AD144">
+        <v>7910</v>
+      </c>
+      <c r="AE144">
+        <v>12252</v>
+      </c>
+      <c r="AF144">
+        <v>9481</v>
+      </c>
+      <c r="AG144">
+        <v>10792</v>
+      </c>
+      <c r="AH144">
+        <v>9432</v>
+      </c>
+      <c r="AI144">
+        <v>8520</v>
+      </c>
+      <c r="AJ144">
+        <v>12027</v>
+      </c>
+      <c r="AK144">
+        <v>9489</v>
+      </c>
+      <c r="AL144">
+        <v>8962</v>
+      </c>
+      <c r="AM144">
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="145" spans="1:39">
+      <c r="A145">
+        <v>11246</v>
+      </c>
+      <c r="B145">
+        <v>262197</v>
+      </c>
+      <c r="C145">
+        <v>36231</v>
+      </c>
+      <c r="D145">
+        <v>32171</v>
+      </c>
+      <c r="E145">
+        <v>12391</v>
+      </c>
+      <c r="F145">
+        <v>8396</v>
+      </c>
+      <c r="G145">
+        <v>201803</v>
+      </c>
+      <c r="H145">
+        <v>2018</v>
+      </c>
+      <c r="I145">
+        <v>3</v>
+      </c>
+      <c r="J145">
+        <v>11788</v>
+      </c>
+      <c r="K145">
+        <v>10737</v>
+      </c>
+      <c r="L145">
+        <v>11329</v>
+      </c>
+      <c r="M145">
+        <v>16072</v>
+      </c>
+      <c r="N145">
+        <v>12493</v>
+      </c>
+      <c r="O145">
+        <v>191772</v>
+      </c>
+      <c r="P145">
+        <v>202486</v>
+      </c>
+      <c r="Q145">
+        <v>201919</v>
+      </c>
+      <c r="R145">
+        <v>236032</v>
+      </c>
+      <c r="S145">
+        <v>237169</v>
+      </c>
+      <c r="T145">
+        <v>23639</v>
+      </c>
+      <c r="U145">
+        <v>27930</v>
+      </c>
+      <c r="V145">
+        <v>30844</v>
+      </c>
+      <c r="W145">
+        <v>41637</v>
+      </c>
+      <c r="X145">
+        <v>29347</v>
+      </c>
+      <c r="Y145">
+        <v>20320</v>
+      </c>
+      <c r="Z145">
+        <v>36513</v>
+      </c>
+      <c r="AA145">
+        <v>18014</v>
+      </c>
+      <c r="AB145">
+        <v>30823</v>
+      </c>
+      <c r="AC145">
+        <v>35208</v>
+      </c>
+      <c r="AD145">
+        <v>6642</v>
+      </c>
+      <c r="AE145">
+        <v>7910</v>
+      </c>
+      <c r="AF145">
+        <v>12252</v>
+      </c>
+      <c r="AG145">
+        <v>8706</v>
+      </c>
+      <c r="AH145">
+        <v>16301</v>
+      </c>
+      <c r="AI145">
+        <v>7276</v>
+      </c>
+      <c r="AJ145">
+        <v>8520</v>
+      </c>
+      <c r="AK145">
+        <v>12027</v>
+      </c>
+      <c r="AL145">
+        <v>9206</v>
+      </c>
+      <c r="AM145">
+        <v>7731</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>